<commit_message>
Improve fixes, shell and templates
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\1_\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31AE150F-BA67-4563-B14D-B74D3D4B7BD4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{16A6FE8B-C988-41B4-B0E4-B99E3A2EBFDB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4590" xr2:uid="{2A8CA9BE-F497-42AD-AC64-2D907311BAC4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
   <si>
     <t>id</t>
   </si>
@@ -99,9 +99,6 @@
     <t>depictionWidth</t>
   </si>
   <si>
-    <t>depictionHighth</t>
-  </si>
-  <si>
     <t>depictionText</t>
   </si>
   <si>
@@ -117,70 +114,136 @@
     <t>depictionLicenseURI</t>
   </si>
   <si>
+    <t>place</t>
+  </si>
+  <si>
+    <t>Aufführungsort</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Friedrichstraße</t>
+  </si>
+  <si>
+    <t>Berliner Adreßbuch : für das Jahr 1906, Berlin: Loewenthal. Digitalisierung: Zentral- und Landesbibliothek Berlin. PURL:  https://digital.zlb.de/viewer/image/34115495_1906/2665/ (letzter Zugriff: 22.01.2026</t>
+  </si>
+  <si>
+    <t>HistoMapBerlin, Landesarchiv Berlin, Straube, Kartenblatt IVA, Ausgabe 1910, EPSG: 3068; https://histomapberlin.de/de/index.html (letzter Zugriff 22.01.2026)</t>
+  </si>
+  <si>
+    <t>Frühere Komische Oper wird abgerissen. In: Neue Zeit. . September 1952, S. 6. https://zefys.staatsbibliothek-berlin.de/list/title/zdb/2612273X/-/1952/26 (letzter Zugriff: 22.01.2026).</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/Alte_Komische_Oper_Berlin</t>
+  </si>
+  <si>
+    <t>Wikipedia</t>
+  </si>
+  <si>
+    <t>Verweigerte Heimat. Léon Jessel (1871-1942), Komponist des »Schwarzwaldmädel«, Albrecht Dümling, Berlin, Lukas Verlag, 2012, S. 159.</t>
+  </si>
+  <si>
+    <t>Berliner Architekturwelt 8, 1906, Heft 11, S. 408</t>
+  </si>
+  <si>
+    <t>CC0 1.0</t>
+  </si>
+  <si>
+    <t>https://creativecommons.org/publicdomain/zero/1.0/</t>
+  </si>
+  <si>
+    <t>https://commons.wikimedia.org/wiki/File:Alte_Komische_Oper_Berlin,_1906.png</t>
+  </si>
+  <si>
+    <t>depictionCreator</t>
+  </si>
+  <si>
+    <t>52.521625</t>
+  </si>
+  <si>
+    <t>13.388228</t>
+  </si>
+  <si>
+    <t>In der Komischen Oper wurde am 25.08.1917 Léon Jessels Operette "Schwarzwaldmädel" uraufgeführt.</t>
+  </si>
+  <si>
+    <t>depictionHight</t>
+  </si>
+  <si>
     <t>Komische Oper</t>
   </si>
   <si>
-    <t>place</t>
-  </si>
-  <si>
-    <t>Aufführungsort</t>
-  </si>
-  <si>
-    <t>Berlin</t>
-  </si>
-  <si>
-    <t>https://d-nb.info/gnd/</t>
-  </si>
-  <si>
-    <t>Friedrichstraße</t>
-  </si>
-  <si>
-    <t>Berliner Adreßbuch : für das Jahr 1906, Berlin: Loewenthal. Digitalisierung: Zentral- und Landesbibliothek Berlin. PURL:  https://digital.zlb.de/viewer/image/34115495_1906/2665/ (letzter Zugriff: 22.01.2026</t>
-  </si>
-  <si>
-    <t>HistoMapBerlin, Landesarchiv Berlin, Straube, Kartenblatt IVA, Ausgabe 1910, EPSG: 3068; https://histomapberlin.de/de/index.html (letzter Zugriff 22.01.2026)</t>
-  </si>
-  <si>
-    <t>Frühere Komische Oper wird abgerissen. In: Neue Zeit. . September 1952, S. 6. https://zefys.staatsbibliothek-berlin.de/list/title/zdb/2612273X/-/1952/26 (letzter Zugriff: 22.01.2026).</t>
-  </si>
-  <si>
-    <t>https://de.wikipedia.org/wiki/Alte_Komische_Oper_Berlin</t>
-  </si>
-  <si>
-    <t>Wikipedia</t>
-  </si>
-  <si>
-    <t>Verweigerte Heimat. Léon Jessel (1871-1942), Komponist des »Schwarzwaldmädel«, Albrecht Dümling, Berlin, Lukas Verlag, 2012, S. 159.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> https://commons.wikimedia.org/wiki/Special:FilePath/Alte_Komische_Oper_Berlin%2C_1906.png?width=270</t>
-  </si>
-  <si>
-    <t>Außenansicht, Komische Oper Berlin, 1906</t>
-  </si>
-  <si>
-    <t>Berliner Architekturwelt 8, 1906, Heft 11, S. 408</t>
-  </si>
-  <si>
-    <t>CC0 1.0</t>
-  </si>
-  <si>
-    <t>https://creativecommons.org/publicdomain/zero/1.0/</t>
-  </si>
-  <si>
-    <t>https://commons.wikimedia.org/wiki/File:Alte_Komische_Oper_Berlin,_1906.png</t>
-  </si>
-  <si>
-    <t>depictionCreator</t>
-  </si>
-  <si>
-    <t>52.521625</t>
-  </si>
-  <si>
-    <t>13.388228</t>
-  </si>
-  <si>
-    <t>In der Komischen Oper wurde am 25.08.1917 Léon Jessels Operette "Schwarzwaldmädel" uraufgeführt.</t>
+    <t>https://d-nb.info/gnd/1224235657</t>
+  </si>
+  <si>
+    <t>https://commons.wikimedia.org/wiki/Special:FilePath/Alte_Komische_Oper_Berlin%2C_1906.png?width=270</t>
+  </si>
+  <si>
+    <t>Außenansicht Komische Oper Berlin, 1906</t>
+  </si>
+  <si>
+    <t>https://d-nb.info/gnd/119285517</t>
+  </si>
+  <si>
+    <t>Léon Jessel</t>
+  </si>
+  <si>
+    <t>person</t>
+  </si>
+  <si>
+    <t>Wohnort</t>
+  </si>
+  <si>
+    <t>Düsseldorfer Straße</t>
+  </si>
+  <si>
+    <t>Verweigerte Heimat. Léon Jessel (1871-1942), Komponist des »Schwarzwaldmädel«, Albrecht Dümling, Berlin, Lukas Verlag, 2012, S. 161.</t>
+  </si>
+  <si>
+    <t>52.49682</t>
+  </si>
+  <si>
+    <t>13.31223</t>
+  </si>
+  <si>
+    <t>1932-1941</t>
+  </si>
+  <si>
+    <t>HistoMapBerlin, Landesarchiv Berlin, K4, Kartenblatt 4146, Ausgabe 1931 + 1941, EPSG: 3068; https://histomapberlin.de/de/index.html (letzter Zugriff 22.01.2026)</t>
+  </si>
+  <si>
+    <t>Verweigerte Heimat. Léon Jessel (1871-1942), Komponist des »Schwarzwaldmädel«, Albrecht Dümling, Berlin, Lukas Verlag, 2012, S. 161-162.</t>
+  </si>
+  <si>
+    <t>leon_jessel</t>
+  </si>
+  <si>
+    <t>https://www.deutsche-digitale-bibliothek.de/person/gnd/119285517</t>
+  </si>
+  <si>
+    <t>Deutsche Digitale Bibliothek</t>
+  </si>
+  <si>
+    <t>Leon Jessel lebte mit kurzer Unterbrechung von 1932 bis 1941 in der Düsseldorfer Straße 47.</t>
+  </si>
+  <si>
+    <t>jpg</t>
+  </si>
+  <si>
+    <t>Léon Jessel um 1933.</t>
+  </si>
+  <si>
+    <t>Wikimedia Commons</t>
+  </si>
+  <si>
+    <t>https://commons.wikimedia.org/wiki/File:Leon%20Jessel.jpg?uselang=de</t>
+  </si>
+  <si>
+    <t>Public Domain</t>
+  </si>
+  <si>
+    <t>https://creativecommons.org/publicdomain/mark/1.0/</t>
   </si>
 </sst>
 </file>
@@ -535,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABFCB451-D26D-4E1F-BE81-8010CAC899BF}">
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:AE3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AE11" sqref="AE11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -620,102 +683,182 @@
         <v>23</v>
       </c>
       <c r="Y1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>28</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>31</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="E2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="G2">
         <v>104</v>
       </c>
       <c r="H2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="K2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="L2">
         <v>1905</v>
       </c>
       <c r="M2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="N2">
         <v>1952</v>
       </c>
       <c r="O2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" t="s">
+        <v>46</v>
+      </c>
+      <c r="U2" t="s">
         <v>38</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="V2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD2" t="s">
         <v>40</v>
       </c>
-      <c r="S2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="T2" t="s">
-        <v>51</v>
-      </c>
-      <c r="U2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="V2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3">
         <v>47</v>
       </c>
-      <c r="AD2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>46</v>
+      <c r="H3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3" t="s">
+        <v>61</v>
+      </c>
+      <c r="P3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>62</v>
+      </c>
+      <c r="R3" t="s">
+        <v>65</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="X3">
+        <v>256</v>
+      </c>
+      <c r="Y3">
+        <v>350</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>